<commit_message>
MAECCO TUMBRADO SA LAYOUT
</commit_message>
<xml_diff>
--- a/NominasMaecco/bin/Debug/Archivos/maecco1.xlsx
+++ b/NominasMaecco/bin/Debug/Archivos/maecco1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\Operadora\OperadoraNominas\OperadoraNominas\bin\Debug\Archivos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\Maecco\NominasMaecco\NominasMaecco\bin\Debug\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Generales" sheetId="2" r:id="rId1"/>
@@ -241,7 +241,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="78">
   <si>
     <t>No. Empleado</t>
   </si>
@@ -466,6 +466,15 @@
   </si>
   <si>
     <t>TAJIN</t>
+  </si>
+  <si>
+    <t>93/002</t>
+  </si>
+  <si>
+    <t>SUBSIDIO</t>
+  </si>
+  <si>
+    <t>Subsidio Causado</t>
   </si>
 </sst>
 </file>
@@ -476,7 +485,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -539,6 +548,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -811,14 +826,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -861,35 +877,48 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="5" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Millares 2 2" xfId="2"/>
     <cellStyle name="Millares 3 2 2" xfId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Normal 4" xfId="3"/>
     <cellStyle name="Normal 7" xfId="1"/>
   </cellStyles>
@@ -1433,40 +1462,40 @@
       <c r="C2" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="33" t="s">
+      <c r="D2" s="31"/>
+      <c r="E2" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="34"/>
+      <c r="F2" s="29"/>
       <c r="G2" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="32"/>
-      <c r="I2" s="33" t="s">
+      <c r="H2" s="31"/>
+      <c r="I2" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="J2" s="34"/>
+      <c r="J2" s="29"/>
       <c r="K2" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="L2" s="32"/>
-      <c r="M2" s="33" t="s">
+      <c r="L2" s="31"/>
+      <c r="M2" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="N2" s="34"/>
+      <c r="N2" s="29"/>
       <c r="O2" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="33" t="s">
+      <c r="P2" s="31"/>
+      <c r="Q2" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="35"/>
-      <c r="V2" s="35"/>
-      <c r="W2" s="34"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="29"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1559,7 +1588,7 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -1604,10 +1633,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="33" t="s">
         <v>60</v>
       </c>
       <c r="E2" s="17" t="s">
@@ -1616,18 +1645,18 @@
       <c r="F2" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="28" t="s">
+      <c r="G2" s="35"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="J2" s="34" t="s">
         <v>63</v>
       </c>
       <c r="K2" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="L2" s="28" t="s">
+      <c r="L2" s="33" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1686,17 +1715,54 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja4"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="43"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="39"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
 </file>
</xml_diff>